<commit_message>
subject 6 - 9
</commit_message>
<xml_diff>
--- a/Subjective_data/postquestionnaire.xlsx
+++ b/Subjective_data/postquestionnaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,20 +794,212 @@
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="Q9">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10">
+        <v>3</v>
+      </c>
+      <c r="Q10">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11">
+        <v>4</v>
+      </c>
+      <c r="Q11">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
subject 10 - 11
</commit_message>
<xml_diff>
--- a/Subjective_data/postquestionnaire.xlsx
+++ b/Subjective_data/postquestionnaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -414,7 +414,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,10 +1006,106 @@
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <v>3</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>5</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13">
+        <v>6</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
subject 17 - 20
</commit_message>
<xml_diff>
--- a/Subjective_data/postquestionnaire.xlsx
+++ b/Subjective_data/postquestionnaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>Valid</t>
   </si>
 </sst>
 </file>
@@ -411,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +474,11 @@
       <c r="Q1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -524,8 +530,11 @@
       <c r="Q2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -577,8 +586,11 @@
       <c r="Q3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -630,8 +642,11 @@
       <c r="Q4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -683,8 +698,11 @@
       <c r="Q5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -736,8 +754,11 @@
       <c r="Q6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -789,8 +810,11 @@
       <c r="Q7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -842,8 +866,11 @@
       <c r="Q8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -895,8 +922,11 @@
       <c r="Q9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -948,8 +978,11 @@
       <c r="Q10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1001,8 +1034,11 @@
       <c r="Q11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1054,8 +1090,11 @@
       <c r="Q12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1107,100 +1146,627 @@
       <c r="Q13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <v>6</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <v>4</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>3</v>
+      </c>
+      <c r="Q16">
+        <v>4</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>4</v>
+      </c>
+      <c r="N17">
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <v>4</v>
+      </c>
+      <c r="P17">
+        <v>4</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>2</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>3</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>6</v>
+      </c>
+      <c r="P19">
+        <v>4</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>5</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>6</v>
+      </c>
+      <c r="P20">
+        <v>4</v>
+      </c>
+      <c r="Q20">
+        <v>6</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>3</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <v>6</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+      <c r="O21">
+        <v>6</v>
+      </c>
+      <c r="P21">
+        <v>5</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>3</v>
+      </c>
+      <c r="N22">
+        <v>3</v>
+      </c>
+      <c r="O22">
+        <v>3</v>
+      </c>
+      <c r="P22">
+        <v>5</v>
+      </c>
+      <c r="Q22">
+        <v>3</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="R29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
subject 21 - 26
</commit_message>
<xml_diff>
--- a/Subjective_data/postquestionnaire.xlsx
+++ b/Subjective_data/postquestionnaire.xlsx
@@ -417,7 +417,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1661,6 +1661,51 @@
       <c r="B23" t="s">
         <v>18</v>
       </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>5</v>
+      </c>
+      <c r="N23">
+        <v>5</v>
+      </c>
+      <c r="O23">
+        <v>5</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+      <c r="Q23">
+        <v>6</v>
+      </c>
       <c r="R23">
         <v>1</v>
       </c>
@@ -1672,6 +1717,51 @@
       <c r="B24" t="s">
         <v>2</v>
       </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24">
+        <v>5</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>5</v>
+      </c>
+      <c r="P24">
+        <v>5</v>
+      </c>
+      <c r="Q24">
+        <v>5</v>
+      </c>
       <c r="R24">
         <v>1</v>
       </c>
@@ -1683,6 +1773,51 @@
       <c r="B25" t="s">
         <v>18</v>
       </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <v>5</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25">
+        <v>4</v>
+      </c>
+      <c r="N25">
+        <v>4</v>
+      </c>
+      <c r="O25">
+        <v>4</v>
+      </c>
+      <c r="P25">
+        <v>5</v>
+      </c>
+      <c r="Q25">
+        <v>4</v>
+      </c>
       <c r="R25">
         <v>1</v>
       </c>
@@ -1694,6 +1829,51 @@
       <c r="B26" t="s">
         <v>2</v>
       </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+      <c r="M26">
+        <v>5</v>
+      </c>
+      <c r="N26">
+        <v>5</v>
+      </c>
+      <c r="O26">
+        <v>3</v>
+      </c>
+      <c r="P26">
+        <v>5</v>
+      </c>
+      <c r="Q26">
+        <v>6</v>
+      </c>
       <c r="R26">
         <v>1</v>
       </c>
@@ -1705,6 +1885,51 @@
       <c r="B27" t="s">
         <v>18</v>
       </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
+      <c r="O27">
+        <v>5</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+      <c r="Q27">
+        <v>6</v>
+      </c>
       <c r="R27">
         <v>1</v>
       </c>
@@ -1715,6 +1940,51 @@
       </c>
       <c r="B28" t="s">
         <v>2</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>4</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+      <c r="N28">
+        <v>3</v>
+      </c>
+      <c r="O28">
+        <v>3</v>
+      </c>
+      <c r="P28">
+        <v>3</v>
+      </c>
+      <c r="Q28">
+        <v>4</v>
       </c>
       <c r="R28">
         <v>1</v>

</xml_diff>

<commit_message>
subject 27 - 29
</commit_message>
<xml_diff>
--- a/Subjective_data/postquestionnaire.xlsx
+++ b/Subjective_data/postquestionnaire.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -417,7 +417,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1997,6 +1997,51 @@
       <c r="B29" t="s">
         <v>18</v>
       </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>2</v>
+      </c>
+      <c r="M29">
+        <v>2</v>
+      </c>
+      <c r="N29">
+        <v>3</v>
+      </c>
+      <c r="O29">
+        <v>3</v>
+      </c>
+      <c r="P29">
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <v>4</v>
+      </c>
       <c r="R29">
         <v>1</v>
       </c>
@@ -2006,7 +2051,52 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
+      </c>
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>4</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30">
+        <v>6</v>
       </c>
       <c r="R30">
         <v>1</v>
@@ -2017,7 +2107,52 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <v>3</v>
+      </c>
+      <c r="O31">
+        <v>4</v>
+      </c>
+      <c r="P31">
+        <v>2</v>
+      </c>
+      <c r="Q31">
+        <v>3</v>
       </c>
       <c r="R31">
         <v>1</v>
@@ -2028,13 +2163,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="R32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
       <c r="R33">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
subject 30 - 31
</commit_message>
<xml_diff>
--- a/Subjective_data/postquestionnaire.xlsx
+++ b/Subjective_data/postquestionnaire.xlsx
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1707,7 @@
         <v>6</v>
       </c>
       <c r="R23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1931,7 +1931,7 @@
         <v>6</v>
       </c>
       <c r="R27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2165,6 +2165,51 @@
       <c r="B32" t="s">
         <v>18</v>
       </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="K32">
+        <v>5</v>
+      </c>
+      <c r="L32">
+        <v>3</v>
+      </c>
+      <c r="M32">
+        <v>5</v>
+      </c>
+      <c r="N32">
+        <v>4</v>
+      </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+      <c r="P32">
+        <v>4</v>
+      </c>
+      <c r="Q32">
+        <v>5</v>
+      </c>
       <c r="R32">
         <v>1</v>
       </c>
@@ -2174,7 +2219,52 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>3</v>
+      </c>
+      <c r="N33">
+        <v>3</v>
+      </c>
+      <c r="O33">
+        <v>4</v>
+      </c>
+      <c r="P33">
+        <v>2</v>
+      </c>
+      <c r="Q33">
+        <v>3</v>
       </c>
       <c r="R33">
         <v>1</v>

</xml_diff>